<commit_message>
Added documentation on a trigger in AccountCharges.
</commit_message>
<xml_diff>
--- a/Physical.xlsx
+++ b/Physical.xlsx
@@ -6232,6 +6232,121 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="140" name="Rectangle 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F2ABF32-5756-45EB-A6E7-901A9824D961}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15573374" y="1285875"/>
+          <a:ext cx="3000375" cy="638175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>TRG: If a card that's linked in AccoundIdentification is expired, an error will raise.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28587</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Connector: Elbow 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BC36F3-30ED-49E4-837B-F1E4355680CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="140" idx="1"/>
+          <a:endCxn id="109" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="14354174" y="1604963"/>
+          <a:ext cx="1219200" cy="1852624"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6558,8 +6673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H8:AJ68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AI21" sqref="AI21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>